<commit_message>
Restored and added full backup project
</commit_message>
<xml_diff>
--- a/resources/questionnaire_codebook_eHealth20252026.xlsx
+++ b/resources/questionnaire_codebook_eHealth20252026.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10520259_polimi_it/Documents/Didattica/eHealth/2025-2026/eHealthProject_20252026/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tauro\OneDrive - Politecnico di Milano\Didattica\eHealth\2025-2026\Questionnaire_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{86973181-51D6-417A-A92C-D27B238C5BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{168D18FB-2652-448D-8324-E2BD3014F63E}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{86973181-51D6-417A-A92C-D27B238C5BDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CB80AA3-D5B3-4815-8C81-C2588F1FFCF3}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{0B0945B9-C174-4759-AFC3-30E0FE949711}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0B0945B9-C174-4759-AFC3-30E0FE949711}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -159,6 +159,9 @@
     <t>Do you use more than one drug at a time?</t>
   </si>
   <si>
+    <t>Are you always able to stop using drugs when you want to? (If never use drugs, answer “Yes”)</t>
+  </si>
+  <si>
     <t>Have you ever had blackouts or flashbacks as a result of drug use?</t>
   </si>
   <si>
@@ -303,24 +306,45 @@
     <t>iat_5</t>
   </si>
   <si>
+    <t>How often do you lose sleep due to late-night internet use?</t>
+  </si>
+  <si>
     <t>iat_6</t>
   </si>
   <si>
+    <t>How often do you find yourself anticipating when you will go online again?</t>
+  </si>
+  <si>
     <t>iat_7</t>
   </si>
   <si>
+    <t>How often do you snap, yell, or act annoyed if someone interrupts you while online?</t>
+  </si>
+  <si>
     <t>iat_8</t>
   </si>
   <si>
+    <t>How often do you find yourself saying 'just a few more minutes' when online?</t>
+  </si>
+  <si>
     <t>iat_9</t>
   </si>
   <si>
+    <t>How often do you try to cut down the amount of time you spend online and fail?</t>
+  </si>
+  <si>
     <t>iat_10</t>
   </si>
   <si>
+    <t>How often do you choose to spend time online instead of spending time with others (family, friends)?</t>
+  </si>
+  <si>
     <t>iat_11</t>
   </si>
   <si>
+    <t>How often do you feel restless, moody, depressed, or irritable when attempting to cut down or stop internet use?</t>
+  </si>
+  <si>
     <t>iat_12</t>
   </si>
   <si>
@@ -330,24 +354,45 @@
     <t>iat_13</t>
   </si>
   <si>
+    <t>How often do you fear that life without the Internet would be boring, empty, or joyless?</t>
+  </si>
+  <si>
     <t>iat_14</t>
   </si>
   <si>
+    <t>How often do you snap, yell, or act annoyed if you are unable to use the Internet?</t>
+  </si>
+  <si>
     <t>iat_15</t>
   </si>
   <si>
+    <t>How often do you fantasize about being online when you are offline?</t>
+  </si>
+  <si>
     <t>iat_16</t>
   </si>
   <si>
+    <t>How often do you lose track of time when online?</t>
+  </si>
+  <si>
     <t>iat_17</t>
   </si>
   <si>
+    <t>How often do your grades or school work suffer because of the amount of time you spend online?</t>
+  </si>
+  <si>
     <t>iat_18</t>
   </si>
   <si>
+    <t>How often do you find yourself staying online longer than you had planned?</t>
+  </si>
+  <si>
     <t>iat_19</t>
   </si>
   <si>
+    <t>How often do you use the Internet as a way of escaping from problems or relieving a dysphoric mood (e.g., feelings of helplessness, guilt, anxiety)?</t>
+  </si>
+  <si>
     <t>iat_20</t>
   </si>
   <si>
@@ -543,6 +588,9 @@
     <t>mspss_11</t>
   </si>
   <si>
+    <t>I can depend on my friends for help if I need it.</t>
+  </si>
+  <si>
     <t>mspss_12</t>
   </si>
   <si>
@@ -610,54 +658,6 @@
   </si>
   <si>
     <t>who5_5</t>
-  </si>
-  <si>
-    <t>How often do your grades or schoolwork suffer because of the amount of time you spend online?</t>
-  </si>
-  <si>
-    <t>How often does your job performance or productivity suffer because of the Internet?</t>
-  </si>
-  <si>
-    <t>How often do you become defensive or secretive when anyone asks you what you do online?</t>
-  </si>
-  <si>
-    <t>How often do you block out disturbing thoughts about your life with soothing thoughts of the Internet?</t>
-  </si>
-  <si>
-    <t>How often do you find that you find yourself anticipating when you will go online again?</t>
-  </si>
-  <si>
-    <t>How often do you fear that life without the Internet would be boring, empty or joyless?</t>
-  </si>
-  <si>
-    <t>How often do you snap, yell or act annoyed if someone bothers you while you are online?</t>
-  </si>
-  <si>
-    <t>How often do you lose sleep due to late night log-ins?</t>
-  </si>
-  <si>
-    <t>How often do you feel preoccupied with the Internet when offline, or fantasize about being online?</t>
-  </si>
-  <si>
-    <t>How often do you find yourself saying “just a few more minutes” when online?</t>
-  </si>
-  <si>
-    <t>How often do you try to cut down the amount of time you spend online?</t>
-  </si>
-  <si>
-    <t>How often do you try to hide how long you’ve been online?</t>
-  </si>
-  <si>
-    <t>How often do you choose to spend more time online over going out with others?</t>
-  </si>
-  <si>
-    <t>How often do you feel depressed, moody or nervous when you are offline, which goes away when you are back online?</t>
-  </si>
-  <si>
-    <t>I can talk about my problems with my friends.</t>
-  </si>
-  <si>
-    <t>Are you unable to stop abusing drugs when you want to? </t>
   </si>
 </sst>
 </file>
@@ -1232,9 +1232,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1272,7 +1272,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1378,7 +1378,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1520,7 +1520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1530,9 +1530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3C76BB-32D7-4EC9-B5FC-EFC12901CC77}">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1769,10 +1767,10 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1783,1116 +1781,1116 @@
         <v>0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>209</v>
+        <v>43</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>194</v>
+        <v>92</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>195</v>
+        <v>96</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>196</v>
+        <v>98</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>197</v>
+        <v>100</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>198</v>
+        <v>102</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>199</v>
+        <v>104</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>201</v>
+        <v>108</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>202</v>
+        <v>110</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>203</v>
+        <v>112</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>204</v>
+        <v>114</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>206</v>
+        <v>118</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>207</v>
+        <v>120</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="B76" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>162</v>
+        <v>177</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D84" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="B91" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="B95" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="B96" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2912,6 +2910,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="eacc3627-6700-4809-ae45-da46c1b77726" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006D6D7AAE0C334644BFBB55DA67EDDC52" ma:contentTypeVersion="18" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="ae07034000f14021f26007fb9bb82e2f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="eacc3627-6700-4809-ae45-da46c1b77726" xmlns:ns4="c28a4d5f-3103-4467-80e0-cfa80f66c90f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="edb5a9b2e5079bb81a72df4e6b3d9fd6" ns3:_="" ns4:_="">
     <xsd:import namespace="eacc3627-6700-4809-ae45-da46c1b77726"/>
@@ -3164,14 +3170,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="eacc3627-6700-4809-ae45-da46c1b77726" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B479DC1-F2D5-4690-A6A1-7158570F75B3}">
   <ds:schemaRefs>
@@ -3181,6 +3179,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C830BA44-80E1-4AA6-8306-70C63A478858}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="c28a4d5f-3103-4467-80e0-cfa80f66c90f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="eacc3627-6700-4809-ae45-da46c1b77726"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F17BFF41-67C0-4967-A00F-2966A4338F18}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3197,21 +3212,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C830BA44-80E1-4AA6-8306-70C63A478858}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="c28a4d5f-3103-4467-80e0-cfa80f66c90f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="eacc3627-6700-4809-ae45-da46c1b77726"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>